<commit_message>
Added logger folder to .gitignore
</commit_message>
<xml_diff>
--- a/src/exportToExcel/Certificate.xlsx
+++ b/src/exportToExcel/Certificate.xlsx
@@ -40,28 +40,28 @@
     <t>course_credit</t>
   </si>
   <si>
-    <t>e8d21d9f-269e-4874-9cf7-0fbb86ccb060</t>
-  </si>
-  <si>
-    <t>Q12345678Q</t>
-  </si>
-  <si>
-    <t>Livia</t>
-  </si>
-  <si>
-    <t>Lika</t>
-  </si>
-  <si>
-    <t>livia@gmail.com</t>
+    <t>cbd81bf4-58cd-4671-931d-9e712a51bb3e</t>
+  </si>
+  <si>
+    <t>Q12312312Q</t>
+  </si>
+  <si>
+    <t>Eda</t>
+  </si>
+  <si>
+    <t>Isaku</t>
+  </si>
+  <si>
+    <t>eda@gmail.com</t>
   </si>
   <si>
     <t>BLSD</t>
   </si>
   <si>
-    <t>2022-05-30</t>
-  </si>
-  <si>
-    <t>9</t>
+    <t>2022-04-22</t>
+  </si>
+  <si>
+    <t>3</t>
   </si>
 </sst>
 </file>

</xml_diff>